<commit_message>
update fix for issue  4-18
</commit_message>
<xml_diff>
--- a/issue tracking-2018-4-20.xlsx
+++ b/issue tracking-2018-4-20.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\fudan\code\CM-master\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{978A4CA4-4A4C-43A5-B853-4C0F60523D3A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="24180" windowHeight="13050" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="2018-3-15-1" sheetId="1" r:id="rId1"/>
@@ -28,14 +22,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2018-3-15-1'!$A$1:$F$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018-3-15-2'!$A$1:$H$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'2018-4-4'!$A$1:$G$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'2018-4-8'!$A$1:$G$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'2018-4-8'!$A$1:$G$10</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143">
   <si>
     <t>序号</t>
   </si>
@@ -108,7 +102,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>课程信息页面中，编辑课程信息时，如果更改课程代码，</t>
     </r>
@@ -117,7 +111,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>我们昨天商量怎么操作来着？？</t>
     </r>
@@ -126,7 +120,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>是不是直接提示错误信息并返回，禁止这个操作。更改课程代码的操作请通过添加课程并删除原记录完成。</t>
     </r>
@@ -135,7 +129,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>我忘记了。</t>
     </r>
@@ -414,6 +408,12 @@
   </si>
   <si>
     <t>教务员页面中，导入和编辑教师信息（修改期望学时）之后强制刷新</t>
+  </si>
+  <si>
+    <t>re-open</t>
+  </si>
+  <si>
+    <t>导入之后强制刷新了，但是编辑教师信息之后没有强制刷新</t>
   </si>
   <si>
     <t>编辑课程信息，编辑成功，注意要重新画所有相关的内容，例如所有拥有同样课程代码的数据条；不然的话就自动F5。</t>
@@ -445,10 +445,10 @@
     <t>负责不同学位课程的教务员之前设置权限，比方说负责本科的教务员老师不可以更改硕士课程。</t>
   </si>
   <si>
+    <t>hold</t>
+  </si>
+  <si>
     <t>当教师期望学时为0时，视作这个老师not available，不应该安排任何课程给他。此处无法用删除这个老师代替，因为假设一个老师第一学期出国，第二学期回来上课，我们就会把第一学期设成0，第二学期正常。所以第一学期不可以排课给他，而且也不可以把这个老师信息管理表里删掉。当然替代方法是从可选教师列表里移除。</t>
-  </si>
-  <si>
-    <t>hold</t>
   </si>
   <si>
     <t>老的copy过来的问题。</t>
@@ -499,47 +499,44 @@
 教师个人页面: 我个人认为没有显示的必要, 所以照旧.</t>
   </si>
   <si>
-    <t>re-open</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>导入之后强制刷新了，但是编辑教师信息之后没有强制刷新</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>hold</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>现在导入的逻辑是什么？如果遇到导入一门课程，它的课程代码在原来数据库里已经存在，是不是会把原来的那条课程记录完全替换成新的导入文件里的内容？但是我发现原来的双代码备注并没有被新导入内容替换。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>open</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>closed</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>已存在的全部重新更新. 双代码没有更新是我漏了这个字段</t>
   </si>
   <si>
     <t>现在的教师信息管理教务员页面中，排课分配好之后，已分配学时，已分配难度的排序好像有点问题，不是完全按照升序或降序排列。</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个因为有些数据是None表格排序区分又问题, 我现在如果是None会默认填个0 这样就可以了</t>
   </si>
   <si>
     <t>确认微调结束之前，步骤四的结果导出不可用</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>导出所有的排课结果</t>
   </si>
   <si>
     <t>教师工号中会含有字母，需要改成字符串格式。注意相应其他逻辑的修改</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂时未发现问题</t>
+  </si>
+  <si>
+    <t>改了</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,8 +553,159 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -570,42 +718,27 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -615,12 +748,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -628,13 +941,255 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -644,7 +1199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -653,52 +1208,90 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -714,19 +1307,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -764,19 +1351,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="图片 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1054,12 +1635,11 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1069,7 +1649,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
@@ -1080,7 +1660,7 @@
     <col min="8" max="8" width="59" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +1686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1116,7 +1696,7 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4">
@@ -1130,7 +1710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1140,7 +1720,7 @@
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4">
@@ -1153,7 +1733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1163,7 +1743,7 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="4">
@@ -1173,7 +1753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1183,7 +1763,7 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4">
@@ -1196,7 +1776,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="6" ht="42.75" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1206,7 +1786,7 @@
       <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="4">
@@ -1219,7 +1799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" ht="28.5" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1229,7 +1809,7 @@
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="4">
@@ -1239,7 +1819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1249,7 +1829,7 @@
       <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="4">
@@ -1262,14 +1842,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="9" ht="28.5" spans="2:8">
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="4">
@@ -1282,7 +1862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="10" ht="99.75" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1292,7 +1872,7 @@
       <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="4">
@@ -1308,7 +1888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" ht="28.5" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1318,7 +1898,7 @@
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="4">
@@ -1328,7 +1908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="12" ht="28.5" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1338,7 +1918,7 @@
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4">
@@ -1351,7 +1931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="13" ht="42.75" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1361,7 +1941,7 @@
       <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="4">
@@ -1377,7 +1957,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="14" ht="28.5" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1387,7 +1967,7 @@
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="4">
@@ -1400,7 +1980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" ht="28.5" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1410,7 +1990,7 @@
       <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="4">
@@ -1420,7 +2000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="16" ht="42.75" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1430,7 +2010,7 @@
       <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="4">
@@ -1440,7 +2020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="17" ht="28.5" spans="1:8">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1450,7 +2030,7 @@
       <c r="C17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="4">
@@ -1460,7 +2040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="18" ht="42.75" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1470,7 +2050,7 @@
       <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="4">
@@ -1481,39 +2061,42 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F19" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <autoFilter ref="A1:F19">
+    <extLst/>
+  </autoFilter>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD73B773-F7B7-455C-8637-B80AF43790D3}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="111.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.25" customWidth="1"/>
+    <col min="2" max="2" width="7.125" customWidth="1"/>
+    <col min="3" max="3" width="53.875" customWidth="1"/>
+    <col min="4" max="4" width="5.25" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="7" max="7" width="111.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1529,7 +2112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="2" ht="57" spans="1:7">
       <c r="A2">
         <v>75</v>
       </c>
@@ -1537,75 +2120,111 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="4">
         <v>43208</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" ht="42.75" spans="1:7">
       <c r="A3">
         <v>76</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>136</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E3" s="4">
         <v>43208</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>77</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>136</v>
+      <c r="C4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E4" s="4">
         <v>43208</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" ht="28.5" spans="1:7">
       <c r="A5">
         <v>78</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>136</v>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="4">
         <v>43210</v>
       </c>
+      <c r="G5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" ht="28.5" spans="1:7">
+      <c r="A6">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4">
+        <v>43197</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="7:7">
+      <c r="G7" s="7" t="s">
+        <v>142</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1615,7 +2234,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.625" style="1" customWidth="1"/>
@@ -1628,7 +2247,7 @@
     <col min="9" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1654,7 +2273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>19</v>
       </c>
@@ -1664,13 +2283,13 @@
       <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="11">
+      <c r="D2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="12">
         <v>43174</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
@@ -1678,7 +2297,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" ht="42.75" spans="1:8">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -1688,18 +2307,18 @@
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="D3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="12">
         <v>43174</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="12"/>
       <c r="H3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" ht="42.75" spans="1:9">
       <c r="A4" s="1">
         <v>21</v>
       </c>
@@ -1709,10 +2328,10 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12">
         <v>43174</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1722,7 +2341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="5" ht="42.75" spans="1:8">
       <c r="A5" s="1">
         <v>22</v>
       </c>
@@ -1732,10 +2351,10 @@
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="D5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="12">
         <v>43174</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1745,7 +2364,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="6" ht="71.25" spans="1:9">
       <c r="A6" s="1">
         <v>23</v>
       </c>
@@ -1755,10 +2374,10 @@
       <c r="C6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="11">
+      <c r="D6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12">
         <v>43174</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -1768,7 +2387,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" ht="28.5" spans="1:8">
       <c r="A7" s="1">
         <v>24</v>
       </c>
@@ -1778,10 +2397,10 @@
       <c r="C7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="11">
+      <c r="D7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="12">
         <v>43174</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1791,7 +2410,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="8" ht="57" spans="1:8">
       <c r="A8" s="1">
         <v>24</v>
       </c>
@@ -1801,17 +2420,17 @@
       <c r="C8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="D8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="12">
         <v>43174</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="9" ht="85.5" spans="1:8">
       <c r="A9" s="1">
         <v>25</v>
       </c>
@@ -1821,10 +2440,10 @@
       <c r="C9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="11">
+      <c r="D9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="12">
         <v>43174</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1835,14 +2454,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H9" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <autoFilter ref="A1:H9">
+    <extLst/>
+  </autoFilter>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1852,7 +2473,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
@@ -1861,7 +2482,7 @@
     <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1881,7 +2502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" ht="42.75" spans="1:7">
       <c r="A2">
         <v>26</v>
       </c>
@@ -1891,7 +2512,7 @@
       <c r="C2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4">
@@ -1902,7 +2523,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" ht="28.5" spans="1:7">
       <c r="A3">
         <v>27</v>
       </c>
@@ -1912,7 +2533,7 @@
       <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4">
@@ -1923,13 +2544,13 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1939,7 +2560,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
@@ -1949,7 +2570,7 @@
     <col min="7" max="7" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1969,7 +2590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>28</v>
       </c>
@@ -1979,7 +2600,7 @@
       <c r="C2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4">
@@ -1990,7 +2611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" ht="28.5" spans="1:7">
       <c r="A3">
         <v>29</v>
       </c>
@@ -2000,7 +2621,7 @@
       <c r="C3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4">
@@ -2010,7 +2631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" ht="28.5" spans="1:7">
       <c r="A4">
         <v>30</v>
       </c>
@@ -2020,7 +2641,7 @@
       <c r="C4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="4">
@@ -2033,7 +2654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>31</v>
       </c>
@@ -2043,7 +2664,7 @@
       <c r="C5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4">
@@ -2053,7 +2674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="6" ht="42.75" spans="1:6">
       <c r="A6">
         <v>32</v>
       </c>
@@ -2063,7 +2684,7 @@
       <c r="C6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="4">
@@ -2073,7 +2694,7 @@
         <v>43179</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>33</v>
       </c>
@@ -2083,7 +2704,7 @@
       <c r="C7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="4">
@@ -2093,7 +2714,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>34</v>
       </c>
@@ -2103,7 +2724,7 @@
       <c r="C8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="4">
@@ -2113,7 +2734,7 @@
         <v>43180</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="9" ht="28.5" spans="1:6">
       <c r="A9">
         <v>35</v>
       </c>
@@ -2123,7 +2744,7 @@
       <c r="C9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="4">
@@ -2133,7 +2754,7 @@
         <v>43180</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" ht="28.5" spans="1:7">
       <c r="A10">
         <v>36</v>
       </c>
@@ -2143,7 +2764,7 @@
       <c r="C10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="4">
@@ -2153,7 +2774,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>37</v>
       </c>
@@ -2163,7 +2784,7 @@
       <c r="C11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="4">
@@ -2174,13 +2795,13 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -2190,7 +2811,7 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
@@ -2200,7 +2821,7 @@
     <col min="7" max="7" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2219,11 +2840,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" ht="42.75" spans="1:7">
       <c r="A2">
         <v>38</v>
       </c>
@@ -2233,7 +2854,7 @@
       <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4">
@@ -2243,7 +2864,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" ht="28.5" spans="1:6">
       <c r="A3">
         <v>39</v>
       </c>
@@ -2253,7 +2874,7 @@
       <c r="C3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4">
@@ -2263,7 +2884,7 @@
         <v>43180</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>40</v>
       </c>
@@ -2273,7 +2894,7 @@
       <c r="C4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="4">
@@ -2283,7 +2904,7 @@
         <v>43180</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>41</v>
       </c>
@@ -2293,7 +2914,7 @@
       <c r="C5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4">
@@ -2304,14 +2925,14 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -2321,7 +2942,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
@@ -2332,7 +2953,7 @@
     <col min="7" max="7" width="10.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2355,7 +2976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" ht="42.75" spans="1:7">
       <c r="A2">
         <v>42</v>
       </c>
@@ -2365,7 +2986,7 @@
       <c r="C2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4">
@@ -2375,7 +2996,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="3" ht="85.5" spans="1:7">
       <c r="A3">
         <v>43</v>
       </c>
@@ -2385,7 +3006,7 @@
       <c r="C3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4">
@@ -2398,7 +3019,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" ht="57" spans="1:7">
       <c r="A4">
         <v>44</v>
       </c>
@@ -2408,7 +3029,7 @@
       <c r="C4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="4">
@@ -2421,7 +3042,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="5" ht="85.5" spans="1:7">
       <c r="A5">
         <v>46</v>
       </c>
@@ -2431,7 +3052,7 @@
       <c r="C5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4">
@@ -2444,7 +3065,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="6" ht="71.25" spans="1:7">
       <c r="A6">
         <v>47</v>
       </c>
@@ -2454,7 +3075,7 @@
       <c r="C6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="4">
@@ -2467,7 +3088,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="7" ht="57" spans="1:7">
       <c r="A7">
         <v>48</v>
       </c>
@@ -2477,7 +3098,7 @@
       <c r="C7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="4">
@@ -2491,13 +3112,13 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -2507,7 +3128,7 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
@@ -2517,7 +3138,7 @@
     <col min="7" max="7" width="34.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2540,7 +3161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="2" ht="57" spans="1:7">
       <c r="A2">
         <v>49</v>
       </c>
@@ -2550,7 +3171,7 @@
       <c r="C2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="4">
@@ -2563,7 +3184,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="3" ht="57" spans="1:7">
       <c r="A3">
         <v>50</v>
       </c>
@@ -2573,7 +3194,7 @@
       <c r="C3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4">
@@ -2586,7 +3207,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" ht="28.5" spans="1:6">
       <c r="A4">
         <v>51</v>
       </c>
@@ -2596,7 +3217,7 @@
       <c r="C4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="4">
@@ -2606,7 +3227,7 @@
         <v>43183</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" ht="28.5" spans="1:7">
       <c r="A5">
         <v>52</v>
       </c>
@@ -2616,7 +3237,7 @@
       <c r="C5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4">
@@ -2630,23 +3251,23 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A13" sqref="$A13:$XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
@@ -2657,7 +3278,7 @@
     <col min="7" max="7" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2680,7 +3301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" ht="28.5" spans="1:7">
       <c r="A2">
         <v>65</v>
       </c>
@@ -2703,7 +3324,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" ht="42.75" spans="1:7">
       <c r="A3">
         <v>57</v>
       </c>
@@ -2723,7 +3344,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" ht="28.5" spans="1:5">
       <c r="A4">
         <v>64</v>
       </c>
@@ -2740,7 +3361,7 @@
         <v>43197</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" ht="28.5" spans="1:7">
       <c r="A5">
         <v>60</v>
       </c>
@@ -2760,7 +3381,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>53</v>
       </c>
@@ -2776,11 +3397,11 @@
       <c r="E6" s="4">
         <v>43194</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" ht="28.5" spans="1:7">
       <c r="A7">
         <v>67</v>
       </c>
@@ -2800,7 +3421,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>66</v>
       </c>
@@ -2818,7 +3439,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="9" ht="28.5" spans="1:5">
       <c r="A9">
         <v>63</v>
       </c>
@@ -2835,7 +3456,7 @@
         <v>43197</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>54</v>
       </c>
@@ -2845,14 +3466,14 @@
       <c r="C10" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="4">
         <v>43194</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" ht="28.5" spans="1:7">
       <c r="A11">
         <v>62</v>
       </c>
@@ -2862,7 +3483,7 @@
       <c r="C11" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="4">
@@ -2872,24 +3493,24 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>55</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="4">
         <v>43194</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>59</v>
       </c>
@@ -2899,17 +3520,17 @@
       <c r="C13" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>132</v>
+      <c r="D13" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="E13" s="4">
         <v>43197</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="G13" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" ht="28.5" spans="1:7">
       <c r="A14">
         <v>58</v>
       </c>
@@ -2917,19 +3538,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="4">
         <v>43197</v>
       </c>
       <c r="G14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" ht="28.5" spans="1:5">
       <c r="A15">
         <v>56</v>
       </c>
@@ -2937,7 +3558,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>9</v>
@@ -2946,7 +3567,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>7</v>
       </c>
@@ -2954,10 +3575,10 @@
         <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>134</v>
+        <v>116</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="E16" s="4">
         <v>43173</v>
@@ -2965,23 +3586,26 @@
       <c r="G16" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G16" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <autoFilter ref="A1:G16">
+    <extLst/>
+  </autoFilter>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="5.125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
@@ -2992,7 +3616,7 @@
     <col min="7" max="7" width="202.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3015,7 +3639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" ht="71.25" spans="1:7">
       <c r="A2">
         <v>45</v>
       </c>
@@ -3023,47 +3647,47 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E2" s="4">
         <v>43180</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" ht="57" spans="1:7">
       <c r="A3">
         <v>68</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>118</v>
+      <c r="C3" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E3" s="4">
         <v>43198</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" ht="28.5" spans="1:5">
       <c r="A4">
         <v>69</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>120</v>
+      <c r="C4" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>9</v>
@@ -3072,15 +3696,15 @@
         <v>43198</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" ht="28.5" spans="1:5">
       <c r="A5">
         <v>70</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>121</v>
+      <c r="C5" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>9</v>
@@ -3089,67 +3713,67 @@
         <v>43198</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" ht="28.5" spans="1:7">
       <c r="A6">
         <v>71</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>137</v>
+      <c r="C6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="4">
         <v>43198</v>
       </c>
       <c r="G6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" ht="42.75" spans="1:7">
       <c r="A7">
         <v>72</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="4">
         <v>43198</v>
       </c>
       <c r="G7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>73</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="4">
         <v>43198</v>
       </c>
       <c r="G8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="99.75" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" ht="99.75" spans="1:7">
       <c r="A9">
         <v>61</v>
       </c>
@@ -3157,19 +3781,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="4">
         <v>43197</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" ht="42.75" spans="1:7">
       <c r="A10">
         <v>74</v>
       </c>
@@ -3177,7 +3801,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>9</v>
@@ -3185,13 +3809,15 @@
       <c r="E10" s="4">
         <v>43199</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>131</v>
+      <c r="G10" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G9" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <autoFilter ref="A1:G10">
+    <extLst/>
+  </autoFilter>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>